<commit_message>
Implementing sale merging logic
</commit_message>
<xml_diff>
--- a/src/data/SALES.xlsx
+++ b/src/data/SALES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\db-update-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\db-update-api\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BD015C-387F-464C-A0DA-322BA3D5113B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3093535-8501-4418-B122-1A45C2C3AECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{689EEC6C-B1FF-4977-B240-5CA88FB0D59D}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{689EEC6C-B1FF-4977-B240-5CA88FB0D59D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>customer</t>
   </si>
@@ -480,7 +480,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,120 +917,48 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2">
-        <v>20059385</v>
-      </c>
-      <c r="D15" s="3">
-        <v>44097.501817129632</v>
-      </c>
-      <c r="E15" s="2">
-        <v>54900</v>
-      </c>
-      <c r="F15" s="4">
-        <v>51003.42</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>52467.49</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2">
-        <v>20059385</v>
-      </c>
-      <c r="D16" s="3">
-        <v>44097.501817129632</v>
-      </c>
-      <c r="E16" s="2">
-        <v>54900</v>
-      </c>
-      <c r="F16" s="4">
-        <v>51003.42</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>52467.49</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="2">
-        <v>20059385</v>
-      </c>
-      <c r="D17" s="3">
-        <v>44097.501817129632</v>
-      </c>
-      <c r="E17" s="2">
-        <v>54900</v>
-      </c>
-      <c r="F17" s="4">
-        <v>51003.42</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>52467.49</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="2">
-        <v>20059385</v>
-      </c>
-      <c r="D18" s="3">
-        <v>44097.501817129632</v>
-      </c>
-      <c r="E18" s="2">
-        <v>54900</v>
-      </c>
-      <c r="F18" s="4">
-        <v>51003.42</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <v>52467.49</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>